<commit_message>
Looking at Champion play rates
Using pandas to determine what the average playrate is of each champion across all toplaners is and how that translates to solo's average play rates.
</commit_message>
<xml_diff>
--- a/workingTables/SoloVsTopAvgs - Copy.xlsx
+++ b/workingTables/SoloVsTopAvgs - Copy.xlsx
@@ -9,18 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28155" windowHeight="12960" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28155" windowHeight="12960" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="SoloVsTopAvgs - Copy" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2072" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2102" uniqueCount="70">
   <si>
     <t>player</t>
   </si>
@@ -136,9 +137,6 @@
     <t>Average Earned Gold Share</t>
   </si>
   <si>
-    <t>Average Team Damage Shate</t>
-  </si>
-  <si>
     <t>Average Total CS</t>
   </si>
   <si>
@@ -175,13 +173,73 @@
     <t>Average CS at 15</t>
   </si>
   <si>
-    <t>Solo Adjusted for Game Length</t>
+    <t>Average Team Damage Share</t>
+  </si>
+  <si>
+    <t>Percent Difference</t>
+  </si>
+  <si>
+    <t>Solo Stats Adjusted for Game Length</t>
+  </si>
+  <si>
+    <t>Games</t>
+  </si>
+  <si>
+    <t>Champion</t>
+  </si>
+  <si>
+    <t>Proportion</t>
+  </si>
+  <si>
+    <t>Renekton</t>
+  </si>
+  <si>
+    <t>Ornn</t>
+  </si>
+  <si>
+    <t>Aatrox</t>
+  </si>
+  <si>
+    <t>Gnar</t>
+  </si>
+  <si>
+    <t>Camille</t>
+  </si>
+  <si>
+    <t>Gangplank</t>
+  </si>
+  <si>
+    <t>Jayce</t>
+  </si>
+  <si>
+    <t>Kennen</t>
+  </si>
+  <si>
+    <t>Sion</t>
+  </si>
+  <si>
+    <t>Sett</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Shen</t>
+  </si>
+  <si>
+    <t>Toplaner</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="172" formatCode="0.0%"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -499,7 +557,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -668,8 +726,72 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -712,8 +834,9 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="7" applyBorder="1"/>
@@ -723,10 +846,35 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="42" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="10" xfId="42" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="7" fillId="3" borderId="10" xfId="7" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="10" xfId="42" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="13" xfId="42" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="14" xfId="42" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -766,25 +914,12 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Percent" xfId="42" builtinId="5"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9797"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9797"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill>
@@ -1366,8 +1501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1032205"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:F20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B25" sqref="B25:C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1376,7 +1511,8 @@
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1389,6 +1525,9 @@
       <c r="D1" s="5" t="s">
         <v>33</v>
       </c>
+      <c r="E1" s="9" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1404,6 +1543,10 @@
         <f>B2-C2</f>
         <v>-0.32689999999999975</v>
       </c>
+      <c r="E2" s="10">
+        <f>1-B2/C2</f>
+        <v>0.12936800031659335</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -1416,8 +1559,12 @@
         <v>2.6728999999999998</v>
       </c>
       <c r="D3" s="2">
-        <f t="shared" ref="D3:D13" si="0">B3-C3</f>
+        <f t="shared" ref="D3:D14" si="0">B3-C3</f>
         <v>0.39380000000000015</v>
+      </c>
+      <c r="E3" s="10">
+        <f t="shared" ref="E3:E14" si="1">1-B3/C3</f>
+        <v>-0.14733061468816655</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1434,6 +1581,10 @@
         <f t="shared" si="0"/>
         <v>-2.9799999999999827E-2</v>
       </c>
+      <c r="E4" s="10">
+        <f t="shared" si="1"/>
+        <v>6.1277785774506155E-3</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -1449,10 +1600,14 @@
         <f t="shared" si="0"/>
         <v>2.658981292379986E-3</v>
       </c>
+      <c r="E5" s="10">
+        <f t="shared" si="1"/>
+        <v>-1.1921743525818984E-2</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="B6" s="1">
         <v>0.23470149170607299</v>
@@ -1464,214 +1619,244 @@
         <f t="shared" si="0"/>
         <v>4.9558631367059847E-3</v>
       </c>
+      <c r="E6" s="10">
+        <f t="shared" si="1"/>
+        <v>-2.1571087848618831E-2</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>43</v>
+      <c r="A7" s="6" t="s">
+        <v>40</v>
       </c>
       <c r="B7" s="1">
+        <v>26770.721699999998</v>
+      </c>
+      <c r="C7" s="1">
+        <v>22212.546200000001</v>
+      </c>
+      <c r="D7" s="3">
+        <f>B7-C7</f>
+        <v>4558.1754999999976</v>
+      </c>
+      <c r="E7" s="10">
+        <f t="shared" si="1"/>
+        <v>-0.20520724904558652</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="1">
         <v>430.58893178303998</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C8" s="1">
         <v>423.253873125864</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D8" s="3">
         <f t="shared" si="0"/>
         <v>7.3350586571759777</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B8" s="1">
+      <c r="E8" s="10">
+        <f t="shared" si="1"/>
+        <v>-1.7330163107555752E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="1">
         <v>3264.7</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C9" s="1">
         <v>3164.1251999999999</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D9" s="3">
         <f t="shared" si="0"/>
         <v>100.57479999999987</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B9" s="1">
+      <c r="E9" s="10">
+        <f t="shared" si="1"/>
+        <v>-3.1785973576519577E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="1">
         <v>4589.8416999999999</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C10" s="1">
         <v>4372.7855</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D10" s="3">
         <f t="shared" si="0"/>
         <v>217.05619999999999</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B10" s="1">
+      <c r="E10" s="10">
+        <f t="shared" si="1"/>
+        <v>-4.9637971036996964E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="1">
         <v>80.275000000000006</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C11" s="1">
         <v>74.885199999999998</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D11" s="3">
         <f t="shared" si="0"/>
         <v>5.3898000000000081</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B11" s="1">
+      <c r="E11" s="10">
+        <f t="shared" si="1"/>
+        <v>-7.1974168460523735E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="1">
         <v>5176.3500000000004</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C12" s="1">
         <v>5033.8770999999997</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D12" s="3">
         <f t="shared" si="0"/>
         <v>142.47290000000066</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B12" s="1">
+      <c r="E12" s="10">
+        <f t="shared" si="1"/>
+        <v>-2.8302816530820785E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="1">
         <v>7271.8167000000003</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C13" s="1">
         <v>6903.8805000000002</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D13" s="3">
         <f t="shared" si="0"/>
         <v>367.9362000000001</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B13" s="1">
+      <c r="E13" s="10">
+        <f t="shared" si="1"/>
+        <v>-5.3294114809779858E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="1">
         <v>128.75</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C14" s="1">
         <v>119.6533</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D14" s="3">
         <f t="shared" si="0"/>
         <v>9.0966999999999985</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="1" t="s">
+      <c r="E14" s="10">
+        <f t="shared" si="1"/>
+        <v>-7.6025483626444013E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B16" s="1">
-        <v>2071.5500000000002</v>
-      </c>
-      <c r="C16" s="1">
-        <v>1974.2519</v>
-      </c>
-      <c r="D16" s="4">
-        <f>B16-C16</f>
-        <v>97.298100000000204</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="F16" s="7"/>
+      <c r="E16" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="F16" s="14"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B17" s="1">
-        <v>276.55</v>
+        <v>2071.5500000000002</v>
       </c>
       <c r="C17" s="1">
-        <v>253.5933</v>
+        <v>1974.2519</v>
       </c>
       <c r="D17" s="4">
         <f>B17-C17</f>
-        <v>22.956700000000012</v>
-      </c>
-      <c r="E17" s="8">
-        <f>B17*($C$16/$B$16)</f>
-        <v>263.56079406483065</v>
-      </c>
-      <c r="F17" s="3">
-        <f>E17-C17</f>
-        <v>9.967494064830646</v>
-      </c>
+        <v>97.298100000000204</v>
+      </c>
+      <c r="E17" s="15"/>
+      <c r="F17" s="16"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B18" s="1">
-        <v>13031.2261</v>
+        <v>276.55</v>
       </c>
       <c r="C18" s="1">
-        <v>12572.723599999999</v>
+        <v>253.5933</v>
       </c>
       <c r="D18" s="4">
         <f>B18-C18</f>
-        <v>458.50250000000051</v>
-      </c>
-      <c r="E18" s="8">
-        <f t="shared" ref="E18:E20" si="1">B18*($C$16/$B$16)</f>
-        <v>12419.165787576736</v>
-      </c>
-      <c r="F18" s="2">
-        <f t="shared" ref="F18:F20" si="2">E18-C18</f>
-        <v>-153.55781242326339</v>
+        <v>22.956700000000012</v>
+      </c>
+      <c r="E18" s="7">
+        <f>B18*($C$17/$B$17)</f>
+        <v>263.56079406483065</v>
+      </c>
+      <c r="F18" s="11">
+        <f>E18-C18</f>
+        <v>9.967494064830646</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B19" s="1">
-        <v>26770.721699999998</v>
+        <v>13031.2261</v>
       </c>
       <c r="C19" s="1">
-        <v>22212.546200000001</v>
+        <v>12572.723599999999</v>
       </c>
       <c r="D19" s="4">
         <f>B19-C19</f>
-        <v>4558.1754999999976</v>
-      </c>
-      <c r="E19" s="8">
-        <f t="shared" si="1"/>
-        <v>25513.334546883358</v>
-      </c>
-      <c r="F19" s="3">
-        <f t="shared" si="2"/>
-        <v>3300.788346883357</v>
+        <v>458.50250000000051</v>
+      </c>
+      <c r="E19" s="7">
+        <f t="shared" ref="E19:E20" si="2">B19*($C$17/$B$17)</f>
+        <v>12419.165787576736</v>
+      </c>
+      <c r="F19" s="11">
+        <f>E19-C19</f>
+        <v>-153.55781242326339</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B20" s="1">
         <v>8840.1391000000003</v>
@@ -1683,12 +1868,12 @@
         <f>B20-C20</f>
         <v>-19.02639999999883</v>
       </c>
-      <c r="E20" s="8">
-        <f t="shared" si="1"/>
+      <c r="E20" s="7">
+        <f t="shared" si="2"/>
         <v>8424.9288766572317</v>
       </c>
-      <c r="F20" s="2">
-        <f t="shared" si="2"/>
+      <c r="F20" s="11">
+        <f t="shared" ref="F19:F20" si="3">E20-C20</f>
         <v>-434.23662334276742</v>
       </c>
     </row>
@@ -22483,7 +22668,10 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D1:D13 D15:D1048576 E14 E16">
+  <mergeCells count="1">
+    <mergeCell ref="E16:F17"/>
+  </mergeCells>
+  <conditionalFormatting sqref="E16 D16:D1048576 D1:D14 E1">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>"&lt;0"</formula>
     </cfRule>
@@ -22491,4 +22679,314 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>24668</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2067</v>
+      </c>
+      <c r="E3" s="17">
+        <f>D3/$A$2</f>
+        <v>8.3792767958488737E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1892</v>
+      </c>
+      <c r="E4" s="17">
+        <f t="shared" ref="E4:E13" si="0">D4/$A$2</f>
+        <v>7.6698556834765688E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1861</v>
+      </c>
+      <c r="E5" s="17">
+        <f t="shared" si="0"/>
+        <v>7.5441868007134746E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C6" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1801</v>
+      </c>
+      <c r="E6" s="17">
+        <f t="shared" si="0"/>
+        <v>7.3009567050429713E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C7" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1377</v>
+      </c>
+      <c r="E7" s="17">
+        <f t="shared" si="0"/>
+        <v>5.582130695638074E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1278</v>
+      </c>
+      <c r="E8" s="17">
+        <f t="shared" si="0"/>
+        <v>5.1808010377817418E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C9" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1275</v>
+      </c>
+      <c r="E9" s="17">
+        <f t="shared" si="0"/>
+        <v>5.1686395329982163E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C10" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" s="1">
+        <v>992</v>
+      </c>
+      <c r="E10" s="17">
+        <f t="shared" si="0"/>
+        <v>4.0214042484190041E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C11" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" s="1">
+        <v>950</v>
+      </c>
+      <c r="E11" s="17">
+        <f t="shared" si="0"/>
+        <v>3.8511431814496511E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C12" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="1">
+        <v>735</v>
+      </c>
+      <c r="E12" s="17">
+        <f t="shared" si="0"/>
+        <v>2.9795686719636776E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" s="1">
+        <f>A2-SUM(D3:D12)</f>
+        <v>10440</v>
+      </c>
+      <c r="E13" s="17">
+        <f t="shared" si="0"/>
+        <v>0.42322036646667749</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C14" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" s="1">
+        <v>24668</v>
+      </c>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>120</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C17" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" s="1">
+        <v>21</v>
+      </c>
+      <c r="E17" s="10">
+        <f>D17/$A$16</f>
+        <v>0.17499999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C18" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" s="1">
+        <v>18</v>
+      </c>
+      <c r="E18" s="10">
+        <f t="shared" ref="E18:E28" si="1">D18/$A$16</f>
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C19" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D19" s="1">
+        <v>13</v>
+      </c>
+      <c r="E19" s="10">
+        <f t="shared" si="1"/>
+        <v>0.10833333333333334</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D20" s="1">
+        <v>11</v>
+      </c>
+      <c r="E20" s="20">
+        <f t="shared" si="1"/>
+        <v>9.166666666666666E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C21" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D21" s="1">
+        <v>10</v>
+      </c>
+      <c r="E21" s="20">
+        <f t="shared" si="1"/>
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C22" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="D22" s="18">
+        <v>7</v>
+      </c>
+      <c r="E22" s="21">
+        <f t="shared" si="1"/>
+        <v>5.8333333333333334E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C23" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D23" s="1">
+        <f>A16-(SUM(D17:D22))</f>
+        <v>40</v>
+      </c>
+      <c r="E23" s="20">
+        <f>D23/$A$16</f>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="24" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C24" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="D24" s="1">
+        <f>SUM(D17:D23)</f>
+        <v>120</v>
+      </c>
+      <c r="E24" s="8"/>
+    </row>
+    <row r="25" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E25" s="8"/>
+    </row>
+    <row r="26" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E26" s="8"/>
+    </row>
+    <row r="27" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E27" s="8"/>
+    </row>
+    <row r="28" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E28" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>